<commit_message>
Added feedback on PD and Arch updates
</commit_message>
<xml_diff>
--- a/Zacher/Feedback.xlsx
+++ b/Zacher/Feedback.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="280" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="156">
   <si>
     <t>Author</t>
   </si>
@@ -392,12 +392,137 @@
   <si>
     <t>Are you sure the DDS signal max freq is 50Khz?</t>
   </si>
+  <si>
+    <t>d7b8fe0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Is the state Indicator Conrtrolled by the State Switch as shown in the Flow diagram or is controled by the micro as shown in the hardware block diagram </t>
+  </si>
+  <si>
+    <t>Clarify which on is correct</t>
+  </si>
+  <si>
+    <t>Master volume block does not appear in this diagram</t>
+  </si>
+  <si>
+    <t>add it to match HWBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hardware Block Diagram </t>
+  </si>
+  <si>
+    <t>What block on the Flow diagram does the ON/OFF switch map to?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Physical Pin interface and Master Volume do not name something you can buy. </t>
+  </si>
+  <si>
+    <t>Rename them to something you can phyiscally get. i.e. how will you implement those two blocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For signals that go to the same I/O, such as PB1, should be shown connected. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redraw siganl to show the connection. This also implies that the pin must be able to operate correctly no matter what signal is flowing through it. For example have you made sure that the ON.OFF switch will not interfere with the programming </t>
+  </si>
+  <si>
+    <t>Great organization :) It is really easy to follow the signal flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How does the power flow through the POT, On/Off Switch and LED. </t>
+  </si>
+  <si>
+    <t>Interface Pinout</t>
+  </si>
+  <si>
+    <t>DDS Pin Interface / DIP Switch is not part of the connector so you do not need to enumerate it here. These connection will be capctured by the schematic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Major Signals list </t>
+  </si>
+  <si>
+    <t>Are you sure the max frequency is for the DDS Tone Output Signal is 32KHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add the Type for each major signal (analog, digital , PWM etc) </t>
+  </si>
+  <si>
+    <t>This makes it easier to understand for the reader. A 1KHz sine wave is different than a 1kHz PWM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculations </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete the loss calculations for the ChebyShev and RC filter. This will give you an idea how much amplification you will need. </t>
+  </si>
+  <si>
+    <t>Product Definition.txt</t>
+  </si>
+  <si>
+    <t>Update Introduction to reflect the current state of the project</t>
+  </si>
+  <si>
+    <t>Do you mean 100mW</t>
+  </si>
+  <si>
+    <t>Chebyshev Low pass filter: "Line Loss must be less than ??100MW??"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amplifier: "200 MW of current" </t>
+  </si>
+  <si>
+    <t>You should use amp for current and watts for power. So do you mean "200 mW of power"?</t>
+  </si>
+  <si>
+    <t>"State: Idle State 
+        Event: Micro Controller is set to Idle"
+Events that where nothing happens can be removed</t>
+  </si>
+  <si>
+    <t>remove this event</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "State: Arduino Frequency Signal Driven State
+        Event: Input is received". Input is received is a vague statement </t>
+  </si>
+  <si>
+    <t>Clarify what you mean</t>
+  </si>
+  <si>
+    <t>"     # The selector connects the chosen Arduino Channel to the micro-controller
+" is a characteristic not a behavior</t>
+  </si>
+  <si>
+    <t>Move to characteristics list</t>
+  </si>
+  <si>
+    <t>Output Signal Controlling States
+    State: EQ slide switch in position A
+        Event: The Switch is in position A
+            # Signal is connected from the from Chebyshev Low Pass filter to amplifier.
+        Event:The Switch is in position B
+            GOTO: EQ slide switch in position B
+    State: EQ slide switch in position B
+        Event: The Switch is in position A
+            GOTO: EQ slide switch in position A
+        Event: The Switch is in position B
+            # Signal is connected from the from Chebyshev Low Pass filter to the 3 band EQ, then the amplifier.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This are accurate which is great  but the infromation it captures is  trivial. Lets talk about what is the best way to capture this information. </t>
+  </si>
+  <si>
+    <t>Arduino &lt;--&gt; Computer Interface command list is missing</t>
+  </si>
+  <si>
+    <t>enumerate the commands you want to be able to send, if any. If you are not going to send any commands the remove this Command Definition</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -461,6 +586,11 @@
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -479,7 +609,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="73">
+  <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -553,8 +683,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -588,9 +726,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="73">
+  <cellStyles count="81">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -634,6 +777,10 @@
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -663,6 +810,10 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1000,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48:C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1842,6 +1993,308 @@
         <v>114</v>
       </c>
     </row>
+    <row r="48" spans="1:5" ht="48">
+      <c r="A48" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="32">
+      <c r="A51" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="32">
+      <c r="A52" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="64">
+      <c r="A53" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="32">
+      <c r="A54" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="37">
+      <c r="A55" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D55" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="32">
+      <c r="A56" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="32">
+      <c r="A57" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E57" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="48">
+      <c r="A58" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="32">
+      <c r="A59" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D59" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="32">
+      <c r="A60" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="32">
+      <c r="A61" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="48">
+      <c r="A62" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="48">
+      <c r="A63" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="48">
+      <c r="A64" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="256">
+      <c r="A65" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="32">
+      <c r="A66" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added feedback on Schematic and layout etc
</commit_message>
<xml_diff>
--- a/Zacher/Feedback.xlsx
+++ b/Zacher/Feedback.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zache_000\Documents\GitHub\Independent\Zacher\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="285" yWindow="0" windowWidth="25605" windowHeight="16065" tabRatio="500"/>
+    <workbookView xWindow="280" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="248">
   <si>
     <t>Author</t>
   </si>
@@ -629,6 +624,163 @@
   </si>
   <si>
     <t>Added.</t>
+  </si>
+  <si>
+    <t>dd443857</t>
+  </si>
+  <si>
+    <t>Feature Block Diagram</t>
+  </si>
+  <si>
+    <t>Only SVG update not the pdf</t>
+  </si>
+  <si>
+    <t>be sure to export to the PDF or just have the svg and use the PDF format only for release</t>
+  </si>
+  <si>
+    <t>Signal flow could be even simpler.</t>
+  </si>
+  <si>
+    <t>Think of was to align blocks (like the computer block, etc) to make it even as easy to read as the Hardware Block diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable Freq Controller text smushed </t>
+  </si>
+  <si>
+    <t>clean this up</t>
+  </si>
+  <si>
+    <t>Signals going to amplifer should be combined since they are the same and the amplifer only has one input</t>
+  </si>
+  <si>
+    <t>Major Components BOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hmm. Using the URL only is dangerous. The URL has a lot of extra information in it so if some one is checking they have to parse it themselve and that is slow and could cause errors. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you can convice me that this will not be a bruden on a reviwer then you can keep it but otherwise you should extract the information from the datasheets and input it into the BOM. </t>
+  </si>
+  <si>
+    <t>Capacitor 22NF
+Capacitor .1uF - these are not major components</t>
+  </si>
+  <si>
+    <t>These parts a jelly bean parts and do not have to be ordered specially</t>
+  </si>
+  <si>
+    <t>The side column make it hard to read</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compress the columns a bit so that you can see </t>
+  </si>
+  <si>
+    <t>Calculations Sheet</t>
+  </si>
+  <si>
+    <t>What are the cutoff frequencies you are using for the LP&lt; HP, and BP filters</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">? </t>
+  </si>
+  <si>
+    <t>Checbyshev Calculations. I do not see them</t>
+  </si>
+  <si>
+    <t>Cable Definition</t>
+  </si>
+  <si>
+    <t>The USB is a premade cable so you do not need to define it</t>
+  </si>
+  <si>
+    <t>You can remove this document. I added the full Cable Definition Template to the Realization folder so you can see what that looks like. You can use it on another project if you need it</t>
+  </si>
+  <si>
+    <t>Eagle Files</t>
+  </si>
+  <si>
+    <t>the Version files (.# files) clog up the folder</t>
+  </si>
+  <si>
+    <t>Add the .# version files to gitignore. See https://git-scm.com/docs/gitignore for information</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schematic </t>
+  </si>
+  <si>
+    <t>Use ground and power symbol not air wires</t>
+  </si>
+  <si>
+    <t>the Symbols are industry standard and it is hard to read without them</t>
+  </si>
+  <si>
+    <t>You must use proper symbol and footprint for the amp and ATTiny</t>
+  </si>
+  <si>
+    <t>I see what you did there and it is quicker but it is a bit of a hack and not acceptable for a professional board. Create the full Device for these parts and replace the headers</t>
+  </si>
+  <si>
+    <t>The schematic is too broken up with air wires</t>
+  </si>
+  <si>
+    <t>using air wires is fine but if you break the schematic up too mych it becomes hard to read. For example U$4 is off the main signal path even though it would be trival to keep it in line</t>
+  </si>
+  <si>
+    <t>Use standard references. For example U is used for ICs not Pots</t>
+  </si>
+  <si>
+    <t>the U$* pattern is the default from Eagle and you should update it to the standard reference letter. See the Schematic Guildelines for details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-Floating aire wire are hard to read. It is very easy to confuse them with just a signal name and not a connection.  For example see S2 - PB1 </t>
+  </si>
+  <si>
+    <t>Air wires should always be showns as floating. Update any air wire that are not floating</t>
+  </si>
+  <si>
+    <t>Match the Schematic Guidelines</t>
+  </si>
+  <si>
+    <t>Schematic Guidelines are not all implemented</t>
+  </si>
+  <si>
+    <t>The schematic could get a bit cramped</t>
+  </si>
+  <si>
+    <t>Make the page as big as you need to make things clear. Use a bigger frame if needed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERC errros not corrected </t>
+  </si>
+  <si>
+    <t>Run ERC and correct errors</t>
+  </si>
+  <si>
+    <t>Layout</t>
+  </si>
+  <si>
+    <t>Board outline is the default</t>
+  </si>
+  <si>
+    <t>Move board outline (Dimension layer) to match what you want</t>
+  </si>
+  <si>
+    <t>Minimize crosses when placing components</t>
+  </si>
+  <si>
+    <t>When you place a component it is much easer to route if the flying wireing do not cross. If they do cross you will have to use via to do the routing. Since we only have two layers if you have too many crosses if you have a lot of crosses it can get hard to route</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will the speaker be part of the board? </t>
+  </si>
+  <si>
+    <t>Flaoting whole to the left of the board? Do you need it</t>
+  </si>
+  <si>
+    <t>Think about single flow on the board and keep parts are connected close to eachother. This makes it easier to route later</t>
   </si>
 </sst>
 </file>
@@ -714,7 +866,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -735,6 +887,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -763,7 +921,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="84">
+  <cellStyleXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -848,8 +1006,20 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -907,8 +1077,44 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="83" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="82" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="83" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="83" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="82" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="82" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="84">
+  <cellStyles count="96">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -956,6 +1162,12 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -989,6 +1201,12 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="81" builtinId="10"/>
     <cellStyle name="Note 2" xfId="82"/>
@@ -1338,28 +1556,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J76"/>
+  <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70:C93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="77.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="83.875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="73.625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="85.25" style="2" customWidth="1"/>
-    <col min="8" max="8" width="83.375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="75.75" style="2" customWidth="1"/>
-    <col min="10" max="10" width="87.375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="59.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="68.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="45.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="85.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="83.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="75.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="87.33203125" style="2" customWidth="1"/>
     <col min="11" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1373,7 +1591,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="15">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1385,7 +1603,7 @@
       </c>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="15">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1394,22 +1612,22 @@
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="6"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" s="1"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="21" t="s">
         <v>4</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1434,14 +1652,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -1458,14 +1676,14 @@
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="12" t="s">
@@ -1482,14 +1700,14 @@
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="12" t="s">
@@ -1506,14 +1724,14 @@
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
     </row>
-    <row r="10" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30">
       <c r="A10" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -1530,14 +1748,14 @@
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
-    <row r="11" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="45">
       <c r="A11" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="12" t="s">
@@ -1554,14 +1772,14 @@
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
     </row>
-    <row r="12" spans="1:10" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="60">
       <c r="A12" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="12" t="s">
@@ -1578,14 +1796,14 @@
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="30">
       <c r="A13" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="12" t="s">
@@ -1602,14 +1820,14 @@
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="30">
       <c r="A14" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="12" t="s">
@@ -1626,14 +1844,14 @@
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
     </row>
-    <row r="15" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="30">
       <c r="A15" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="12" t="s">
@@ -1650,14 +1868,14 @@
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="A16" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -1674,14 +1892,14 @@
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
     </row>
-    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="60">
       <c r="A17" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="12" t="s">
@@ -1698,14 +1916,14 @@
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="12" t="s">
@@ -1722,14 +1940,14 @@
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="30">
       <c r="A19" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="12" t="s">
@@ -1746,14 +1964,14 @@
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
     </row>
-    <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="45">
       <c r="A20" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="12" t="s">
@@ -1774,14 +1992,14 @@
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="30">
       <c r="A21" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="12" t="s">
@@ -1796,14 +2014,14 @@
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D22" s="12" t="s">
@@ -1820,14 +2038,14 @@
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="12" t="s">
@@ -1844,14 +2062,14 @@
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D24" s="12" t="s">
@@ -1868,14 +2086,14 @@
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
     </row>
-    <row r="25" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="45">
       <c r="A25" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="16" t="s">
@@ -1894,396 +2112,384 @@
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="15" t="s">
+    <row r="26" spans="1:10" s="28" customFormat="1">
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C27" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D27" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="E27" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F27" s="12" t="s">
         <v>127</v>
-      </c>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>128</v>
       </c>
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10">
       <c r="A28" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="E28" s="12"/>
+        <v>170</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>171</v>
+      </c>
       <c r="F28" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10">
       <c r="A29" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>81</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="E29" s="12"/>
       <c r="F29" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="30">
       <c r="A30" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="E30" s="12"/>
+        <v>61</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>81</v>
+      </c>
       <c r="F30" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10">
       <c r="A31" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="15" t="s">
+      <c r="C31" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>83</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="E31" s="12"/>
       <c r="F31" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10">
       <c r="A32" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C32" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>173</v>
+        <v>82</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>174</v>
+        <v>132</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10">
       <c r="A33" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C33" s="15" t="s">
+      <c r="C33" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>74</v>
+        <v>173</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F33" s="12" t="s">
-        <v>133</v>
+        <v>174</v>
       </c>
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
     </row>
-    <row r="34" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10">
       <c r="A34" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F34" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="30">
       <c r="A35" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E35" s="12"/>
+        <v>76</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>77</v>
+      </c>
       <c r="F35" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10">
       <c r="A36" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>65</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="E36" s="12"/>
       <c r="F36" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10">
       <c r="A37" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10">
       <c r="A38" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D38" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>193</v>
+      <c r="D38" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>137</v>
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="30">
       <c r="A39" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D39" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>138</v>
+      <c r="D39" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>193</v>
       </c>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
     </row>
-    <row r="40" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10">
       <c r="A40" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C40" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="E40" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="F40" s="14" t="s">
-        <v>134</v>
+      <c r="D40" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>138</v>
       </c>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="45">
       <c r="A41" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D41" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>71</v>
+        <v>177</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>194</v>
+        <v>134</v>
       </c>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" ht="30">
       <c r="A42" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D42" s="14" t="s">
-        <v>70</v>
+        <v>178</v>
       </c>
       <c r="E42" s="14" t="s">
         <v>71</v>
@@ -2296,599 +2502,1013 @@
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10">
       <c r="A43" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C43" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D43" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12" t="s">
-        <v>139</v>
+      <c r="D43" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F43" s="14" t="s">
+        <v>194</v>
       </c>
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10">
       <c r="A44" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>60</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="E44" s="12"/>
       <c r="F44" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10">
       <c r="A45" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10">
       <c r="A46" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B46" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C46" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>179</v>
+        <v>69</v>
       </c>
       <c r="F46" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
     </row>
-    <row r="47" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10">
       <c r="A47" s="15" t="s">
         <v>1</v>
       </c>
       <c r="B47" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="15" t="s">
+      <c r="C47" s="5" t="s">
         <v>57</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>180</v>
+        <v>80</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>88</v>
+        <v>179</v>
       </c>
       <c r="F47" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
     </row>
-    <row r="48" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="G48" s="19"/>
-      <c r="H48" s="19"/>
+    <row r="48" spans="1:10" ht="30">
+      <c r="A48" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A49" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="B49" s="18" t="s">
+    <row r="49" spans="1:10" s="28" customFormat="1">
+      <c r="A49" s="23"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="27"/>
+      <c r="J49" s="27"/>
+    </row>
+    <row r="50" spans="1:10" ht="45">
+      <c r="A50" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C49" s="15" t="s">
+      <c r="C50" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D49" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E49" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="F49" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A50" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="15" t="s">
-        <v>93</v>
-      </c>
       <c r="D50" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="E50" s="14"/>
+        <v>181</v>
+      </c>
+      <c r="E50" s="14" t="s">
+        <v>94</v>
+      </c>
       <c r="F50" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G50" s="19"/>
       <c r="H50" s="19"/>
       <c r="I50" s="14"/>
       <c r="J50" s="14"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A51" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B51" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C51" s="15" t="s">
+    <row r="51" spans="1:10">
+      <c r="A51" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="E51" s="14"/>
+        <v>95</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>96</v>
+      </c>
       <c r="F51" s="14" t="s">
-        <v>146</v>
+        <v>195</v>
       </c>
       <c r="G51" s="19"/>
       <c r="H51" s="19"/>
       <c r="I51" s="14"/>
       <c r="J51" s="14"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10">
       <c r="A52" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B52" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C52" s="15" t="s">
+      <c r="C52" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D52" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="E52" s="14" t="s">
-        <v>149</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="E52" s="14"/>
       <c r="F52" s="14" t="s">
-        <v>182</v>
+        <v>145</v>
       </c>
       <c r="G52" s="19"/>
       <c r="H52" s="19"/>
       <c r="I52" s="14"/>
       <c r="J52" s="14"/>
     </row>
-    <row r="53" spans="1:10" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10">
       <c r="A53" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B53" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="15" t="s">
+      <c r="C53" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D53" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>150</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="E53" s="14"/>
       <c r="F53" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G53" s="19"/>
       <c r="H53" s="19"/>
       <c r="I53" s="14"/>
       <c r="J53" s="14"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="30">
       <c r="A54" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B54" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="15" t="s">
+      <c r="C54" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D54" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="E54" s="14"/>
+        <v>99</v>
+      </c>
+      <c r="E54" s="14" t="s">
+        <v>149</v>
+      </c>
       <c r="F54" s="14" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="G54" s="19"/>
       <c r="H54" s="19"/>
       <c r="I54" s="14"/>
       <c r="J54" s="14"/>
     </row>
-    <row r="55" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" ht="45">
       <c r="A55" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B55" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="C55" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D55" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E55" s="14"/>
+        <v>100</v>
+      </c>
+      <c r="E55" s="14" t="s">
+        <v>150</v>
+      </c>
       <c r="F55" s="14" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="G55" s="19"/>
       <c r="H55" s="19"/>
       <c r="I55" s="14"/>
       <c r="J55" s="14"/>
     </row>
-    <row r="56" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" ht="30">
       <c r="A56" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B56" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C56" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C56" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D56" s="14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E56" s="14"/>
       <c r="F56" s="14" t="s">
-        <v>187</v>
+        <v>148</v>
       </c>
       <c r="G56" s="19"/>
       <c r="H56" s="19"/>
       <c r="I56" s="14"/>
       <c r="J56" s="14"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" ht="45">
       <c r="A57" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B57" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="C57" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C57" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D57" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="E57" s="14" t="s">
-        <v>106</v>
-      </c>
+        <v>151</v>
+      </c>
+      <c r="E57" s="14"/>
       <c r="F57" s="14" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G57" s="19"/>
       <c r="H57" s="19"/>
       <c r="I57" s="14"/>
       <c r="J57" s="14"/>
     </row>
-    <row r="58" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" ht="30">
       <c r="A58" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B58" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="C58" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D58" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E58" s="14"/>
       <c r="F58" s="14" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="G58" s="19"/>
       <c r="H58" s="19"/>
       <c r="I58" s="14"/>
       <c r="J58" s="14"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" ht="30">
       <c r="A59" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B59" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C59" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C59" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D59" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="E59" s="14"/>
+        <v>152</v>
+      </c>
+      <c r="E59" s="14" t="s">
+        <v>106</v>
+      </c>
       <c r="F59" s="14" t="s">
-        <v>127</v>
+        <v>188</v>
       </c>
       <c r="G59" s="19"/>
       <c r="H59" s="19"/>
       <c r="I59" s="14"/>
       <c r="J59" s="14"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" ht="30">
       <c r="A60" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="C60" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D60" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="E60" s="14" t="s">
-        <v>111</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="E60" s="14"/>
       <c r="F60" s="14" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="G60" s="19"/>
       <c r="H60" s="19"/>
       <c r="I60" s="14"/>
       <c r="J60" s="14"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10">
       <c r="A61" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B61" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C61" s="15" t="s">
+      <c r="C61" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D61" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>114</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="E61" s="14"/>
       <c r="F61" s="14" t="s">
-        <v>184</v>
+        <v>127</v>
       </c>
       <c r="G61" s="19"/>
       <c r="H61" s="19"/>
       <c r="I61" s="14"/>
       <c r="J61" s="14"/>
     </row>
-    <row r="62" spans="1:10" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10">
       <c r="A62" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B62" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D62" s="14" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F62" s="14" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="G62" s="19"/>
       <c r="H62" s="19"/>
       <c r="I62" s="14"/>
       <c r="J62" s="14"/>
     </row>
-    <row r="63" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" ht="30">
       <c r="A63" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B63" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C63" s="15" t="s">
+      <c r="C63" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F63" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G63" s="19"/>
       <c r="H63" s="19"/>
       <c r="I63" s="14"/>
       <c r="J63" s="14"/>
     </row>
-    <row r="64" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" ht="45">
       <c r="A64" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B64" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C64" s="15" t="s">
+      <c r="C64" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F64" s="14" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G64" s="19"/>
       <c r="H64" s="19"/>
       <c r="I64" s="14"/>
       <c r="J64" s="14"/>
     </row>
-    <row r="65" spans="1:10" ht="236.25" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" ht="30">
       <c r="A65" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B65" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C65" s="15" t="s">
+      <c r="C65" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="F65" s="14" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G65" s="19"/>
       <c r="H65" s="19"/>
       <c r="I65" s="14"/>
       <c r="J65" s="14"/>
     </row>
-    <row r="66" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" ht="45">
       <c r="A66" s="20" t="s">
         <v>1</v>
       </c>
       <c r="B66" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C66" s="15" t="s">
+      <c r="C66" s="5" t="s">
         <v>93</v>
       </c>
       <c r="D66" s="14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F66" s="14" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G66" s="19"/>
       <c r="H66" s="19"/>
       <c r="I66" s="14"/>
       <c r="J66" s="14"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C67" s="9"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C68" s="9"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C69" s="9"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C70" s="9"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C71" s="9"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C72" s="9"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C73" s="9"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C74" s="9"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C75" s="9"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C76" s="9"/>
+    <row r="67" spans="1:10" ht="240">
+      <c r="A67" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B67" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="E67" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F67" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="G67" s="19"/>
+      <c r="H67" s="19"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+    </row>
+    <row r="68" spans="1:10" ht="30">
+      <c r="A68" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B68" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F68" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="G68" s="19"/>
+      <c r="H68" s="19"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+    </row>
+    <row r="69" spans="1:10" s="28" customFormat="1">
+      <c r="A69" s="31"/>
+      <c r="B69" s="31"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="27"/>
+      <c r="E69" s="27"/>
+      <c r="F69" s="27"/>
+      <c r="G69" s="32"/>
+      <c r="H69" s="32"/>
+      <c r="I69" s="27"/>
+      <c r="J69" s="27"/>
+    </row>
+    <row r="70" spans="1:10" ht="36">
+      <c r="A70" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="36">
+      <c r="A71" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="36">
+      <c r="A73" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="54">
+      <c r="A74" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="36">
+      <c r="A75" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="36">
+      <c r="A77" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="54">
+      <c r="A79" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="36">
+      <c r="A80" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="54">
+      <c r="A82" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="36">
+      <c r="A83" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C83" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="54">
+      <c r="A84" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="54">
+      <c r="A85" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="36">
+      <c r="A87" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C87" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C89" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="72">
+      <c r="A90" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C92" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="54">
+      <c r="A93" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>247</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Added feedback on Schematic and Layout
</commit_message>
<xml_diff>
--- a/Zacher/Feedback.xlsx
+++ b/Zacher/Feedback.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="294">
   <si>
     <t>Author</t>
   </si>
@@ -781,6 +781,144 @@
   </si>
   <si>
     <t>Think about single flow on the board and keep parts are connected close to eachother. This makes it easier to route later</t>
+  </si>
+  <si>
+    <t>ce91bfa</t>
+  </si>
+  <si>
+    <t>Schematic</t>
+  </si>
+  <si>
+    <t>What is the function of C1? If it is bypass for the Arduino that is already handled on the Uno Board is self. Have extra bypass is not bad but not absolutly necessary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What happens to Uno_Tone_Master if all S2 switch are opened. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is good practice to have input voltage defined for all states so it may be a good idea to add a pull done on Uno_Tone_Master to deal with this case. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">C2 is in a non-standard configuration with GND on top. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is not a big deal but it will make it easier to read if you flip the VCC and GND pins on the synbol. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All Capcaitors are shown polarized? </t>
+  </si>
+  <si>
+    <t>Will they all be polarized? If not then you should used the non-polarized symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What is the purpose of R1? As it is shown right now it will bypass the LED which mean the LED would be dim or not light up. </t>
+  </si>
+  <si>
+    <t>Signal Flow is very clear</t>
+  </si>
+  <si>
+    <t>Great :)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name and Rev on Pin Layer </t>
+  </si>
+  <si>
+    <t>Move to Symbol Layer</t>
+  </si>
+  <si>
+    <t>Guideline mismatch: Reference leter for Switches, Pot, Connector</t>
+  </si>
+  <si>
+    <t>Match the Guideline!</t>
+  </si>
+  <si>
+    <t>Guideline mismatch:Standard Passive not called out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C1 looks like it is for bypass bit it is unclear </t>
+  </si>
+  <si>
+    <t>if so move it to connect to 5V going into the op-amp pin 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guideline Mismatch: Unclear if there are special passive or not </t>
+  </si>
+  <si>
+    <t>Add callout for voltage etc for any special components</t>
+  </si>
+  <si>
+    <t>NOT ALL NETS NAMED!!!</t>
+  </si>
+  <si>
+    <t>NAME ALL NETS!!</t>
+  </si>
+  <si>
+    <t>Guideline mistmach: Four way connection on 3Band_Equ</t>
+  </si>
+  <si>
+    <t>Use two junctions to show connections</t>
+  </si>
+  <si>
+    <t>ERC not cleared!!</t>
+  </si>
+  <si>
+    <t>CLEAR ERC before you submit your work!!</t>
+  </si>
+  <si>
+    <t>Good not on Speaker calling out J1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Board outline oversized </t>
+  </si>
+  <si>
+    <t>Used the space or reduce the size of the board. It is confusing if you have unused space letft there for some reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guideline Mismatch: Display on Part Reference and not Value </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Ground plane </t>
+  </si>
+  <si>
+    <t>Ground trace used and not ground Plane</t>
+  </si>
+  <si>
+    <t>No need to restrict your self to Arduino sheild outline</t>
+  </si>
+  <si>
+    <t>You can use a bigger board if needed to make things easier to use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pots placed hapazardly </t>
+  </si>
+  <si>
+    <t>They are put where they fit as opposed to what will be easiest for the user. Consider how a user would want them placed and shift accordinly</t>
+  </si>
+  <si>
+    <t>Gudeline Mistmach: References different size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRC not cleared </t>
+  </si>
+  <si>
+    <t>Clear the DRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creative comon notes not placed </t>
+  </si>
+  <si>
+    <t>Move them to where it will be clean as opposed to having them randoming placed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Over all the routing is pretty messy </t>
+  </si>
+  <si>
+    <t>Clean up routing so signal flow is clear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No callout for testing. </t>
+  </si>
+  <si>
+    <t>Add test point and solder jumpers on at least major signals</t>
   </si>
 </sst>
 </file>
@@ -866,7 +1004,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -896,6 +1034,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -921,7 +1065,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="96">
+  <cellStyleXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1018,8 +1162,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1113,8 +1283,11 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="82" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="96">
+  <cellStyles count="122">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1168,6 +1341,19 @@
     <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1207,6 +1393,19 @@
     <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="81" builtinId="10"/>
     <cellStyle name="Note 2" xfId="82"/>
@@ -1556,10 +1755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J93"/>
+  <dimension ref="A1:J120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70:C93"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1591,7 +1790,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:10" ht="15">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1603,7 +1802,7 @@
       </c>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:10">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -3294,7 +3493,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="81" spans="1:5">
+    <row r="81" spans="1:10">
       <c r="A81" s="20" t="s">
         <v>1</v>
       </c>
@@ -3311,7 +3510,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="54">
+    <row r="82" spans="1:10" ht="54">
       <c r="A82" s="20" t="s">
         <v>1</v>
       </c>
@@ -3328,7 +3527,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="36">
+    <row r="83" spans="1:10" ht="36">
       <c r="A83" s="20" t="s">
         <v>1</v>
       </c>
@@ -3345,7 +3544,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="54">
+    <row r="84" spans="1:10" ht="54">
       <c r="A84" s="20" t="s">
         <v>1</v>
       </c>
@@ -3362,7 +3561,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="54">
+    <row r="85" spans="1:10" ht="54">
       <c r="A85" s="20" t="s">
         <v>1</v>
       </c>
@@ -3379,7 +3578,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="86" spans="1:5">
+    <row r="86" spans="1:10">
       <c r="A86" s="20" t="s">
         <v>1</v>
       </c>
@@ -3396,7 +3595,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="36">
+    <row r="87" spans="1:10" ht="36">
       <c r="A87" s="20" t="s">
         <v>1</v>
       </c>
@@ -3413,7 +3612,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="88" spans="1:5">
+    <row r="88" spans="1:10">
       <c r="A88" s="20" t="s">
         <v>1</v>
       </c>
@@ -3430,7 +3629,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="89" spans="1:5">
+    <row r="89" spans="1:10">
       <c r="A89" s="20" t="s">
         <v>1</v>
       </c>
@@ -3447,7 +3646,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="72">
+    <row r="90" spans="1:10" ht="72">
       <c r="A90" s="20" t="s">
         <v>1</v>
       </c>
@@ -3464,7 +3663,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="91" spans="1:5">
+    <row r="91" spans="1:10">
       <c r="A91" s="20" t="s">
         <v>1</v>
       </c>
@@ -3478,7 +3677,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="92" spans="1:5">
+    <row r="92" spans="1:10">
       <c r="A92" s="20" t="s">
         <v>1</v>
       </c>
@@ -3492,7 +3691,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="54">
+    <row r="93" spans="1:10" ht="54">
       <c r="A93" s="20" t="s">
         <v>1</v>
       </c>
@@ -3504,6 +3703,448 @@
       </c>
       <c r="D93" s="2" t="s">
         <v>247</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" s="28" customFormat="1">
+      <c r="A94" s="31"/>
+      <c r="B94" s="31"/>
+      <c r="C94" s="24"/>
+      <c r="D94" s="27"/>
+      <c r="E94" s="27"/>
+      <c r="F94" s="27"/>
+      <c r="G94" s="32"/>
+      <c r="H94" s="32"/>
+      <c r="I94" s="27"/>
+      <c r="J94" s="27"/>
+    </row>
+    <row r="95" spans="1:10" ht="54">
+      <c r="A95" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="54">
+      <c r="A96" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="36">
+      <c r="A97" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="36">
+      <c r="A98" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="54">
+      <c r="A99" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="A102" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="A103" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="36">
+      <c r="A104" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D104" s="33" t="s">
+        <v>262</v>
+      </c>
+      <c r="E104" s="33" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
+      <c r="A105" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D105" s="33" t="s">
+        <v>264</v>
+      </c>
+      <c r="E105" s="33" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="36">
+      <c r="A106" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D106" s="33" t="s">
+        <v>267</v>
+      </c>
+      <c r="E106" s="33" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
+      <c r="A107" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D107" s="33" t="s">
+        <v>269</v>
+      </c>
+      <c r="E107" s="33" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D108" s="33" t="s">
+        <v>271</v>
+      </c>
+      <c r="E108" s="33" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="A109" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D109" s="33" t="s">
+        <v>273</v>
+      </c>
+      <c r="E109" s="33" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D111" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="E111" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="36">
+      <c r="A112" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D113" s="33" t="s">
+        <v>278</v>
+      </c>
+      <c r="E113" s="33" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
+      <c r="A114" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="36">
+      <c r="A116" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="A117" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D117" s="33" t="s">
+        <v>285</v>
+      </c>
+      <c r="E117" s="33" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
+      <c r="A118" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="36">
+      <c r="A119" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
+      <c r="A120" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E120" s="2" t="s">
+        <v>291</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Task Enumeration and Feedback
</commit_message>
<xml_diff>
--- a/Zacher/Feedback.xlsx
+++ b/Zacher/Feedback.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zache_000\Documents\GitHub\Independent\Zacher\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="398">
   <si>
     <t>Author</t>
   </si>
@@ -1023,6 +1018,219 @@
   </si>
   <si>
     <t>Value removed</t>
+  </si>
+  <si>
+    <t>becd0aa</t>
+  </si>
+  <si>
+    <t>Align Computer block with main signal path</t>
+  </si>
+  <si>
+    <t>Computer block is off main signal path making the diagram harder to read</t>
+  </si>
+  <si>
+    <t>Introduction Good</t>
+  </si>
+  <si>
+    <t>Product Characteristics: Operating Temperature seems a little low. What if they take itoutside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature 2: - Operate 60-90 F is redundant </t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>Feature 3 good</t>
+  </si>
+  <si>
+    <t>Feature 4 Less than 50MW power draw?</t>
+  </si>
+  <si>
+    <t>do you mean mW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature 4 :Output in the physical spectrum? This is unclear </t>
+  </si>
+  <si>
+    <t>Clarify what you mean by this. Does it mean that you are using a LED?</t>
+  </si>
+  <si>
+    <t>Feature 6: Good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feature 7: Line Loss must be less than 100mW ? </t>
+  </si>
+  <si>
+    <t>Maybe this should be removed. Or changed to voltage</t>
+  </si>
+  <si>
+    <t>Feature 8 Good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feaure 10 Good </t>
+  </si>
+  <si>
+    <t>Feature 11: Good</t>
+  </si>
+  <si>
+    <t>Behavior Definition: Product State: Separation between Input and Output states is unclear</t>
+  </si>
+  <si>
+    <t>Show the separation some how</t>
+  </si>
+  <si>
+    <t>Detailed Behavior is good</t>
+  </si>
+  <si>
+    <t>Interface is good</t>
+  </si>
+  <si>
+    <t>Synchronize with Hardware Block Diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firmware Block Diagram </t>
+  </si>
+  <si>
+    <t>Not made</t>
+  </si>
+  <si>
+    <t>If you are not going to make one then it should be removed</t>
+  </si>
+  <si>
+    <t>Hardware blockdiagram</t>
+  </si>
+  <si>
+    <t>Great</t>
+  </si>
+  <si>
+    <t>Check LED block is connected correctly</t>
+  </si>
+  <si>
+    <t>Major Signal List: Good</t>
+  </si>
+  <si>
+    <t>Interface List: Speaker Pinout missing</t>
+  </si>
+  <si>
+    <t>For completeness add it in. This is something the a person assembling the PCB would need to know</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Budget: Slide Switch does not draw power </t>
+  </si>
+  <si>
+    <t>Remove from list</t>
+  </si>
+  <si>
+    <t>Product Architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slide Swithc does not draw power </t>
+  </si>
+  <si>
+    <t>remove ground and power symbol from that block</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove from list. </t>
+  </si>
+  <si>
+    <t>Current Budget: EQ does not draw power. Match the HWBD</t>
+  </si>
+  <si>
+    <t>Current Budget: Pushbutton only on momentarily so duty cycle is &lt;1%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current Budget: Pot is on all the time and will not draw 100mA. </t>
+  </si>
+  <si>
+    <t>Update duty cycle and recaculate current draw based on resistance of the pot you chose. Also check the voltage range for the pot</t>
+  </si>
+  <si>
+    <t>Calculations: Colors are good but the cels are to large making it hard to read</t>
+  </si>
+  <si>
+    <t>Use text wrap or not to make the cells smaller. Try to get the width to one screen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculations: The DIV/0 error are distracting. </t>
+  </si>
+  <si>
+    <t>Remove calc if you are not going to use it</t>
+  </si>
+  <si>
+    <t>Fill out</t>
+  </si>
+  <si>
+    <t>Still Incomplete</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Arduino failed to open file</t>
+  </si>
+  <si>
+    <t>Remove white space from name</t>
+  </si>
+  <si>
+    <t>Code incomplete</t>
+  </si>
+  <si>
+    <t>Add input side and clean up comments</t>
+  </si>
+  <si>
+    <t>Add test points to major signal</t>
+  </si>
+  <si>
+    <t>Not voltage test points</t>
+  </si>
+  <si>
+    <t>Part number should be in the Value field</t>
+  </si>
+  <si>
+    <t>For LED put the part number in the value field and use the Label command for the color. Same for non-standard passive packages like the Inductors</t>
+  </si>
+  <si>
+    <t>Great net names!</t>
+  </si>
+  <si>
+    <t>Approval of errors is good</t>
+  </si>
+  <si>
+    <t>5V trace is fine but be careful not to cut the ground plane too much with traces. The more you cut it the less effective it is</t>
+  </si>
+  <si>
+    <t>Refernces for pots etc are covered by the part</t>
+  </si>
+  <si>
+    <t>Move them so they would be visible after the part is placed</t>
+  </si>
+  <si>
+    <t>Signal flow is easy to follow</t>
+  </si>
+  <si>
+    <t>Is R29 redundant since you have the final volume pot</t>
+  </si>
+  <si>
+    <t>Remove is so</t>
+  </si>
+  <si>
+    <t>Bypass caps are great</t>
+  </si>
+  <si>
+    <t>Bring Up Change List</t>
+  </si>
+  <si>
+    <t>Update and complete</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rework tracking </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incomplete </t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1377,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="122">
+  <cellStyleXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1254,6 +1462,26 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1409,7 +1637,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="122">
+  <cellStyles count="142">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1476,6 +1704,16 @@
     <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1528,6 +1766,16 @@
     <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="81" builtinId="10"/>
     <cellStyle name="Note 2" xfId="82"/>
@@ -1877,29 +2125,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:J132"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:J165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119:F119"/>
+    <sheetView tabSelected="1" topLeftCell="A152" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="B166" sqref="B166"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="18" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="68.5" style="2" customWidth="1"/>
-    <col min="6" max="6" width="45.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="85.125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="83.375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="75.625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="87.375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="45.83203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="85.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="83.33203125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="75.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="87.33203125" style="2" customWidth="1"/>
     <col min="11" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1913,7 +2161,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1925,7 +2173,7 @@
       </c>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -1934,15 +2182,15 @@
       </c>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" s="6"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="A5" s="1"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="A6" s="9" t="s">
         <v>5</v>
       </c>
@@ -1974,7 +2222,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="A7" s="10" t="s">
         <v>1</v>
       </c>
@@ -1998,7 +2246,7 @@
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10">
       <c r="A8" s="10" t="s">
         <v>1</v>
       </c>
@@ -2022,7 +2270,7 @@
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="A9" s="10" t="s">
         <v>1</v>
       </c>
@@ -2046,7 +2294,7 @@
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
     </row>
-    <row r="10" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="30">
       <c r="A10" s="10" t="s">
         <v>1</v>
       </c>
@@ -2070,7 +2318,7 @@
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
     </row>
-    <row r="11" spans="1:10" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="45">
       <c r="A11" s="10" t="s">
         <v>1</v>
       </c>
@@ -2094,7 +2342,7 @@
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
     </row>
-    <row r="12" spans="1:10" ht="63" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="60">
       <c r="A12" s="10" t="s">
         <v>1</v>
       </c>
@@ -2118,7 +2366,7 @@
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
     </row>
-    <row r="13" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="30">
       <c r="A13" s="10" t="s">
         <v>1</v>
       </c>
@@ -2142,7 +2390,7 @@
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
     </row>
-    <row r="14" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="30">
       <c r="A14" s="10" t="s">
         <v>1</v>
       </c>
@@ -2166,7 +2414,7 @@
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
     </row>
-    <row r="15" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="30">
       <c r="A15" s="10" t="s">
         <v>1</v>
       </c>
@@ -2190,7 +2438,7 @@
       <c r="I15" s="13"/>
       <c r="J15" s="13"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="A16" s="10" t="s">
         <v>1</v>
       </c>
@@ -2214,7 +2462,7 @@
       <c r="I16" s="13"/>
       <c r="J16" s="13"/>
     </row>
-    <row r="17" spans="1:10" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" ht="45">
       <c r="A17" s="10" t="s">
         <v>1</v>
       </c>
@@ -2238,7 +2486,7 @@
       <c r="I17" s="13"/>
       <c r="J17" s="13"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10">
       <c r="A18" s="10" t="s">
         <v>1</v>
       </c>
@@ -2262,7 +2510,7 @@
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
     </row>
-    <row r="19" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" ht="30">
       <c r="A19" s="10" t="s">
         <v>1</v>
       </c>
@@ -2286,7 +2534,7 @@
       <c r="I19" s="13"/>
       <c r="J19" s="13"/>
     </row>
-    <row r="20" spans="1:10" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="45">
       <c r="A20" s="10" t="s">
         <v>1</v>
       </c>
@@ -2314,7 +2562,7 @@
       <c r="I20" s="13"/>
       <c r="J20" s="13"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10">
       <c r="A21" s="10" t="s">
         <v>1</v>
       </c>
@@ -2336,7 +2584,7 @@
       <c r="I21" s="13"/>
       <c r="J21" s="13"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10">
       <c r="A22" s="10" t="s">
         <v>1</v>
       </c>
@@ -2360,7 +2608,7 @@
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10">
       <c r="A23" s="10" t="s">
         <v>1</v>
       </c>
@@ -2384,7 +2632,7 @@
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10">
       <c r="A24" s="10" t="s">
         <v>1</v>
       </c>
@@ -2408,7 +2656,7 @@
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
     </row>
-    <row r="25" spans="1:10" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" ht="45">
       <c r="A25" s="14" t="s">
         <v>1</v>
       </c>
@@ -2434,7 +2682,7 @@
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
     </row>
-    <row r="26" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" s="27" customFormat="1">
       <c r="A26" s="22"/>
       <c r="B26" s="22"/>
       <c r="C26" s="23"/>
@@ -2446,7 +2694,7 @@
       <c r="I26" s="26"/>
       <c r="J26" s="26"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10">
       <c r="A27" s="14" t="s">
         <v>1</v>
       </c>
@@ -2470,7 +2718,7 @@
       <c r="I27" s="13"/>
       <c r="J27" s="13"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10">
       <c r="A28" s="14" t="s">
         <v>1</v>
       </c>
@@ -2494,7 +2742,7 @@
       <c r="I28" s="13"/>
       <c r="J28" s="13"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10">
       <c r="A29" s="14" t="s">
         <v>1</v>
       </c>
@@ -2516,7 +2764,7 @@
       <c r="I29" s="13"/>
       <c r="J29" s="13"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10">
       <c r="A30" s="14" t="s">
         <v>1</v>
       </c>
@@ -2540,7 +2788,7 @@
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10">
       <c r="A31" s="14" t="s">
         <v>1</v>
       </c>
@@ -2562,7 +2810,7 @@
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10">
       <c r="A32" s="14" t="s">
         <v>1</v>
       </c>
@@ -2586,7 +2834,7 @@
       <c r="I32" s="13"/>
       <c r="J32" s="13"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10">
       <c r="A33" s="14" t="s">
         <v>1</v>
       </c>
@@ -2610,7 +2858,7 @@
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10">
       <c r="A34" s="14" t="s">
         <v>1</v>
       </c>
@@ -2634,7 +2882,7 @@
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
     </row>
-    <row r="35" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" ht="30">
       <c r="A35" s="14" t="s">
         <v>1</v>
       </c>
@@ -2658,7 +2906,7 @@
       <c r="I35" s="13"/>
       <c r="J35" s="13"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10">
       <c r="A36" s="14" t="s">
         <v>1</v>
       </c>
@@ -2680,7 +2928,7 @@
       <c r="I36" s="13"/>
       <c r="J36" s="13"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10">
       <c r="A37" s="14" t="s">
         <v>1</v>
       </c>
@@ -2704,7 +2952,7 @@
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10">
       <c r="A38" s="14" t="s">
         <v>1</v>
       </c>
@@ -2728,7 +2976,7 @@
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
     </row>
-    <row r="39" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" ht="30">
       <c r="A39" s="14" t="s">
         <v>1</v>
       </c>
@@ -2752,7 +3000,7 @@
       <c r="I39" s="13"/>
       <c r="J39" s="13"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10">
       <c r="A40" s="14" t="s">
         <v>1</v>
       </c>
@@ -2776,7 +3024,7 @@
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
     </row>
-    <row r="41" spans="1:10" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" ht="45">
       <c r="A41" s="14" t="s">
         <v>1</v>
       </c>
@@ -2800,7 +3048,7 @@
       <c r="I41" s="13"/>
       <c r="J41" s="13"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10">
       <c r="A42" s="14" t="s">
         <v>1</v>
       </c>
@@ -2824,7 +3072,7 @@
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10">
       <c r="A43" s="14" t="s">
         <v>1</v>
       </c>
@@ -2848,7 +3096,7 @@
       <c r="I43" s="13"/>
       <c r="J43" s="13"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10">
       <c r="A44" s="14" t="s">
         <v>1</v>
       </c>
@@ -2870,7 +3118,7 @@
       <c r="I44" s="13"/>
       <c r="J44" s="13"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10">
       <c r="A45" s="14" t="s">
         <v>1</v>
       </c>
@@ -2894,7 +3142,7 @@
       <c r="I45" s="13"/>
       <c r="J45" s="13"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10">
       <c r="A46" s="14" t="s">
         <v>1</v>
       </c>
@@ -2918,7 +3166,7 @@
       <c r="I46" s="13"/>
       <c r="J46" s="13"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10">
       <c r="A47" s="14" t="s">
         <v>1</v>
       </c>
@@ -2942,7 +3190,7 @@
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
     </row>
-    <row r="48" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" ht="30">
       <c r="A48" s="14" t="s">
         <v>1</v>
       </c>
@@ -2966,7 +3214,7 @@
       <c r="I48" s="13"/>
       <c r="J48" s="13"/>
     </row>
-    <row r="49" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" s="27" customFormat="1">
       <c r="A49" s="22"/>
       <c r="B49" s="22"/>
       <c r="C49" s="23"/>
@@ -2978,7 +3226,7 @@
       <c r="I49" s="26"/>
       <c r="J49" s="26"/>
     </row>
-    <row r="50" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="30">
       <c r="A50" s="17" t="s">
         <v>1</v>
       </c>
@@ -3002,7 +3250,7 @@
       <c r="I50" s="13"/>
       <c r="J50" s="13"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10">
       <c r="A51" s="17" t="s">
         <v>1</v>
       </c>
@@ -3026,7 +3274,7 @@
       <c r="I51" s="13"/>
       <c r="J51" s="13"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10">
       <c r="A52" s="19" t="s">
         <v>1</v>
       </c>
@@ -3048,7 +3296,7 @@
       <c r="I52" s="13"/>
       <c r="J52" s="13"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10">
       <c r="A53" s="19" t="s">
         <v>1</v>
       </c>
@@ -3070,7 +3318,7 @@
       <c r="I53" s="13"/>
       <c r="J53" s="13"/>
     </row>
-    <row r="54" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" ht="30">
       <c r="A54" s="19" t="s">
         <v>1</v>
       </c>
@@ -3094,7 +3342,7 @@
       <c r="I54" s="13"/>
       <c r="J54" s="13"/>
     </row>
-    <row r="55" spans="1:10" ht="63" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" ht="45">
       <c r="A55" s="19" t="s">
         <v>1</v>
       </c>
@@ -3118,7 +3366,7 @@
       <c r="I55" s="13"/>
       <c r="J55" s="13"/>
     </row>
-    <row r="56" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" ht="30">
       <c r="A56" s="19" t="s">
         <v>1</v>
       </c>
@@ -3140,7 +3388,7 @@
       <c r="I56" s="13"/>
       <c r="J56" s="13"/>
     </row>
-    <row r="57" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" ht="30">
       <c r="A57" s="19" t="s">
         <v>1</v>
       </c>
@@ -3162,7 +3410,7 @@
       <c r="I57" s="13"/>
       <c r="J57" s="13"/>
     </row>
-    <row r="58" spans="1:10" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" ht="30">
       <c r="A58" s="19" t="s">
         <v>1</v>
       </c>
@@ -3184,7 +3432,7 @@
       <c r="I58" s="13"/>
       <c r="J58" s="13"/>
     </row>
-    <row r="59" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" ht="30">
       <c r="A59" s="19" t="s">
         <v>1</v>
       </c>
@@ -3208,7 +3456,7 @@
       <c r="I59" s="13"/>
       <c r="J59" s="13"/>
     </row>
-    <row r="60" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" ht="30">
       <c r="A60" s="19" t="s">
         <v>1</v>
       </c>
@@ -3230,7 +3478,7 @@
       <c r="I60" s="13"/>
       <c r="J60" s="13"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10">
       <c r="A61" s="19" t="s">
         <v>1</v>
       </c>
@@ -3252,7 +3500,7 @@
       <c r="I61" s="13"/>
       <c r="J61" s="13"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10">
       <c r="A62" s="19" t="s">
         <v>1</v>
       </c>
@@ -3276,7 +3524,7 @@
       <c r="I62" s="13"/>
       <c r="J62" s="13"/>
     </row>
-    <row r="63" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" ht="30">
       <c r="A63" s="19" t="s">
         <v>1</v>
       </c>
@@ -3300,7 +3548,7 @@
       <c r="I63" s="13"/>
       <c r="J63" s="13"/>
     </row>
-    <row r="64" spans="1:10" ht="47.25" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" ht="45">
       <c r="A64" s="19" t="s">
         <v>1</v>
       </c>
@@ -3324,7 +3572,7 @@
       <c r="I64" s="13"/>
       <c r="J64" s="13"/>
     </row>
-    <row r="65" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" ht="30">
       <c r="A65" s="19" t="s">
         <v>1</v>
       </c>
@@ -3348,7 +3596,7 @@
       <c r="I65" s="13"/>
       <c r="J65" s="13"/>
     </row>
-    <row r="66" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" ht="30">
       <c r="A66" s="19" t="s">
         <v>1</v>
       </c>
@@ -3372,7 +3620,7 @@
       <c r="I66" s="13"/>
       <c r="J66" s="13"/>
     </row>
-    <row r="67" spans="1:10" ht="236.25" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" ht="225">
       <c r="A67" s="19" t="s">
         <v>1</v>
       </c>
@@ -3396,7 +3644,7 @@
       <c r="I67" s="13"/>
       <c r="J67" s="13"/>
     </row>
-    <row r="68" spans="1:10" ht="31.5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" ht="30">
       <c r="A68" s="19" t="s">
         <v>1</v>
       </c>
@@ -3420,7 +3668,7 @@
       <c r="I68" s="13"/>
       <c r="J68" s="13"/>
     </row>
-    <row r="69" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" s="27" customFormat="1">
       <c r="A69" s="30"/>
       <c r="B69" s="30"/>
       <c r="C69" s="23"/>
@@ -3432,7 +3680,7 @@
       <c r="I69" s="26"/>
       <c r="J69" s="26"/>
     </row>
-    <row r="70" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" ht="36">
       <c r="A70" s="19" t="s">
         <v>1</v>
       </c>
@@ -3449,7 +3697,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="71" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" ht="36">
       <c r="A71" s="19" t="s">
         <v>1</v>
       </c>
@@ -3466,7 +3714,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10">
       <c r="A72" s="19" t="s">
         <v>1</v>
       </c>
@@ -3483,7 +3731,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="73" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" ht="36">
       <c r="A73" s="19" t="s">
         <v>1</v>
       </c>
@@ -3498,7 +3746,7 @@
       </c>
       <c r="E73" s="32"/>
     </row>
-    <row r="74" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" ht="54">
       <c r="A74" s="19" t="s">
         <v>1</v>
       </c>
@@ -3515,7 +3763,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" ht="36">
       <c r="A75" s="19" t="s">
         <v>1</v>
       </c>
@@ -3532,7 +3780,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10">
       <c r="A76" s="19" t="s">
         <v>1</v>
       </c>
@@ -3549,7 +3797,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10">
       <c r="A77" s="19" t="s">
         <v>1</v>
       </c>
@@ -3566,7 +3814,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10">
       <c r="A78" s="19" t="s">
         <v>1</v>
       </c>
@@ -3583,7 +3831,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" ht="54">
       <c r="A79" s="19" t="s">
         <v>1</v>
       </c>
@@ -3603,7 +3851,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" ht="36">
       <c r="A80" s="19" t="s">
         <v>1</v>
       </c>
@@ -3623,7 +3871,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="81" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10">
       <c r="A81" s="19" t="s">
         <v>1</v>
       </c>
@@ -3643,7 +3891,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" ht="54">
       <c r="A82" s="19" t="s">
         <v>1</v>
       </c>
@@ -3663,7 +3911,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="83" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" ht="36">
       <c r="A83" s="19" t="s">
         <v>1</v>
       </c>
@@ -3683,7 +3931,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" ht="54">
       <c r="A84" s="19" t="s">
         <v>1</v>
       </c>
@@ -3703,7 +3951,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" ht="36">
       <c r="A85" s="19" t="s">
         <v>1</v>
       </c>
@@ -3723,7 +3971,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10">
       <c r="A86" s="19" t="s">
         <v>1</v>
       </c>
@@ -3743,7 +3991,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" ht="36">
       <c r="A87" s="19" t="s">
         <v>1</v>
       </c>
@@ -3763,7 +4011,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10">
       <c r="A88" s="19" t="s">
         <v>1</v>
       </c>
@@ -3783,7 +4031,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10">
       <c r="A89" s="19" t="s">
         <v>1</v>
       </c>
@@ -3803,7 +4051,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="90" spans="1:10" ht="75" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" ht="72">
       <c r="A90" s="19" t="s">
         <v>1</v>
       </c>
@@ -3823,7 +4071,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10">
       <c r="A91" s="19" t="s">
         <v>1</v>
       </c>
@@ -3840,7 +4088,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="92" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" ht="36">
       <c r="A92" s="19" t="s">
         <v>1</v>
       </c>
@@ -3857,7 +4105,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" ht="36">
       <c r="A93" s="19" t="s">
         <v>1</v>
       </c>
@@ -3874,7 +4122,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="94" spans="1:10" s="27" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" s="27" customFormat="1">
       <c r="A94" s="30"/>
       <c r="B94" s="33"/>
       <c r="C94" s="34"/>
@@ -3886,7 +4134,7 @@
       <c r="I94" s="26"/>
       <c r="J94" s="26"/>
     </row>
-    <row r="95" spans="1:10" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" ht="54">
       <c r="A95" s="37" t="s">
         <v>1</v>
       </c>
@@ -3903,7 +4151,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="96" spans="1:10" ht="112.5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" ht="108">
       <c r="A96" s="37" t="s">
         <v>1</v>
       </c>
@@ -3923,7 +4171,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="36">
       <c r="A97" s="37" t="s">
         <v>1</v>
       </c>
@@ -3943,7 +4191,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="36">
       <c r="A98" s="37" t="s">
         <v>1</v>
       </c>
@@ -3963,7 +4211,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="36">
       <c r="A99" s="37" t="s">
         <v>1</v>
       </c>
@@ -3980,7 +4228,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6">
       <c r="A100" s="37" t="s">
         <v>1</v>
       </c>
@@ -4000,7 +4248,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6">
       <c r="A101" s="37" t="s">
         <v>1</v>
       </c>
@@ -4020,7 +4268,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6">
       <c r="A102" s="37" t="s">
         <v>1</v>
       </c>
@@ -4040,7 +4288,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6">
       <c r="A103" s="37" t="s">
         <v>1</v>
       </c>
@@ -4051,7 +4299,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" ht="36">
       <c r="A104" s="38" t="s">
         <v>1</v>
       </c>
@@ -4071,7 +4319,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="36">
       <c r="A105" s="38" t="s">
         <v>1</v>
       </c>
@@ -4091,7 +4339,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" ht="36">
       <c r="A106" s="38" t="s">
         <v>1</v>
       </c>
@@ -4111,7 +4359,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6">
       <c r="A107" s="38" t="s">
         <v>1</v>
       </c>
@@ -4131,7 +4379,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6">
       <c r="A108" s="38" t="s">
         <v>1</v>
       </c>
@@ -4151,7 +4399,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6">
       <c r="A109" s="38" t="s">
         <v>1</v>
       </c>
@@ -4171,7 +4419,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6">
       <c r="A110" s="37" t="s">
         <v>1</v>
       </c>
@@ -4191,7 +4439,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6">
       <c r="A111" s="37" t="s">
         <v>1</v>
       </c>
@@ -4211,7 +4459,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="36">
       <c r="A112" s="37" t="s">
         <v>1</v>
       </c>
@@ -4231,7 +4479,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10">
       <c r="A113" s="38" t="s">
         <v>1</v>
       </c>
@@ -4251,7 +4499,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" ht="36">
       <c r="A114" s="37" t="s">
         <v>1</v>
       </c>
@@ -4271,7 +4519,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" ht="36">
       <c r="A115" s="37" t="s">
         <v>1</v>
       </c>
@@ -4291,7 +4539,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" ht="36">
       <c r="A116" s="37" t="s">
         <v>1</v>
       </c>
@@ -4311,7 +4559,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" ht="36">
       <c r="A117" s="38" t="s">
         <v>1</v>
       </c>
@@ -4331,7 +4579,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10">
       <c r="A118" s="37" t="s">
         <v>1</v>
       </c>
@@ -4351,7 +4599,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" ht="36">
       <c r="A119" s="39" t="s">
         <v>1</v>
       </c>
@@ -4369,7 +4617,7 @@
       </c>
       <c r="F119" s="32"/>
     </row>
-    <row r="120" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" ht="36">
       <c r="A120" s="37" t="s">
         <v>1</v>
       </c>
@@ -4389,7 +4637,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10">
       <c r="A121" s="32" t="s">
         <v>322</v>
       </c>
@@ -4405,24 +4653,380 @@
       <c r="E121" s="32"/>
       <c r="F121" s="32"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D128" s="32"/>
-    </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D129" s="32"/>
-    </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D130" s="32"/>
-    </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D131" s="32"/>
-    </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D132" s="32"/>
+    <row r="122" spans="1:10" s="27" customFormat="1">
+      <c r="A122" s="30"/>
+      <c r="B122" s="33"/>
+      <c r="C122" s="34"/>
+      <c r="D122" s="35"/>
+      <c r="E122" s="35"/>
+      <c r="F122" s="26"/>
+      <c r="G122" s="31"/>
+      <c r="H122" s="31"/>
+      <c r="I122" s="26"/>
+      <c r="J122" s="26"/>
+    </row>
+    <row r="123" spans="1:10">
+      <c r="A123" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
+      <c r="B124" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="36">
+      <c r="B125" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
+      <c r="B126" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
+      <c r="B127" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
+      <c r="B128" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D128" s="32" t="s">
+        <v>335</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5">
+      <c r="B129" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D129" s="32" t="s">
+        <v>337</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5">
+      <c r="B130" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5">
+      <c r="B131" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D131" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="132" spans="2:5">
+      <c r="B132" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D132" s="32" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5">
+      <c r="B133" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5">
+      <c r="B134" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5" ht="36">
+      <c r="B135" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5">
+      <c r="B136" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5">
+      <c r="B137" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5">
+      <c r="B138" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5">
+      <c r="D139" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5">
+      <c r="B140" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5">
+      <c r="B141" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D141" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5">
+      <c r="D142" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="143" spans="2:5">
+      <c r="D143" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="144" spans="2:5">
+      <c r="B144" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="145" spans="2:5" ht="36">
+      <c r="D145" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="146" spans="2:5">
+      <c r="D146" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="147" spans="2:5">
+      <c r="D147" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="148" spans="2:5">
+      <c r="D148" s="2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="149" spans="2:5" ht="36">
+      <c r="D149" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="150" spans="2:5" ht="36">
+      <c r="D150" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="151" spans="2:5">
+      <c r="D151" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="152" spans="2:5" ht="36">
+      <c r="B152" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="153" spans="2:5">
+      <c r="B153" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="154" spans="2:5">
+      <c r="D154" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="155" spans="2:5">
+      <c r="B155" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D155" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="156" spans="2:5">
+      <c r="D156" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E156" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="157" spans="2:5" ht="54">
+      <c r="D157" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E157" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="158" spans="2:5">
+      <c r="D158" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="159" spans="2:5">
+      <c r="D159" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="160" spans="2:5" ht="36">
+      <c r="B160" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D160" s="2" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="161" spans="2:5">
+      <c r="D161" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="162" spans="2:5">
+      <c r="D162" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="163" spans="2:5">
+      <c r="D163" s="2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="164" spans="2:5">
+      <c r="B164" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="D164" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="165" spans="2:5">
+      <c r="B165" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="D165" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>394</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Revert "Revert "feedback change""
This reverts commit 57809904ec71e7adb62262ae291d4527a86e2073.
</commit_message>
<xml_diff>
--- a/Zacher/Feedback.xlsx
+++ b/Zacher/Feedback.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="327">
   <si>
     <t>Author</t>
   </si>
@@ -869,9 +869,6 @@
     <t>CLEAR ERC before you submit your work!!</t>
   </si>
   <si>
-    <t xml:space="preserve">Board outline oversized </t>
-  </si>
-  <si>
     <t>Used the space or reduce the size of the board. It is confusing if you have unused space letft there for some reason</t>
   </si>
   <si>
@@ -1010,9 +1007,6 @@
     <t>Took into consideration in the newest revision current revision.</t>
   </si>
   <si>
-    <t>smach comand and change all size at once would be cool</t>
-  </si>
-  <si>
     <t>schematic</t>
   </si>
   <si>
@@ -1023,6 +1017,12 @@
   </si>
   <si>
     <t>added a comment to call out the standard passives</t>
+  </si>
+  <si>
+    <t>group comand to make all the refrences the same size</t>
+  </si>
+  <si>
+    <t>Value removed</t>
   </si>
 </sst>
 </file>
@@ -1880,8 +1880,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="D113" sqref="D113"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119:F119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -3600,7 +3600,7 @@
         <v>219</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -3620,7 +3620,7 @@
         <v>222</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -3700,7 +3700,7 @@
         <v>229</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -3720,7 +3720,7 @@
         <v>233</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
@@ -3740,7 +3740,7 @@
         <v>234</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -3760,7 +3760,7 @@
         <v>237</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
@@ -3780,7 +3780,7 @@
         <v>239</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
@@ -3800,7 +3800,7 @@
         <v>242</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="75" x14ac:dyDescent="0.3">
@@ -3820,7 +3820,7 @@
         <v>244</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
@@ -3837,7 +3837,7 @@
         <v>245</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -3854,7 +3854,7 @@
         <v>246</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -3900,7 +3900,7 @@
         <v>250</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="112.5" x14ac:dyDescent="0.3">
@@ -3920,7 +3920,7 @@
         <v>252</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -3940,7 +3940,7 @@
         <v>254</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -3960,7 +3960,7 @@
         <v>256</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -3977,7 +3977,7 @@
         <v>257</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3997,7 +3997,7 @@
         <v>259</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -4068,7 +4068,7 @@
         <v>263</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -4088,7 +4088,7 @@
         <v>263</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -4108,7 +4108,7 @@
         <v>268</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -4128,7 +4128,7 @@
         <v>270</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -4148,7 +4148,7 @@
         <v>272</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -4168,7 +4168,7 @@
         <v>274</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -4182,13 +4182,13 @@
         <v>248</v>
       </c>
       <c r="D110" s="36" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E110" s="36" t="s">
         <v>259</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -4202,13 +4202,13 @@
         <v>248</v>
       </c>
       <c r="D111" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E111" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="E111" s="2" t="s">
-        <v>292</v>
-      </c>
       <c r="F111" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -4222,32 +4222,34 @@
         <v>248</v>
       </c>
       <c r="D112" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="E112" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="E112" s="2" t="s">
-        <v>276</v>
-      </c>
       <c r="F112" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B113" s="32" t="s">
+      <c r="B113" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C113" s="32" t="s">
+      <c r="C113" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D113" s="32" t="s">
-        <v>277</v>
-      </c>
-      <c r="E113" s="32" t="s">
+      <c r="D113" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="E113" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="F113" s="32"/>
+      <c r="F113" s="2" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="114" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A114" s="37" t="s">
@@ -4260,16 +4262,16 @@
         <v>248</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A115" s="37" t="s">
         <v>1</v>
       </c>
@@ -4280,13 +4282,13 @@
         <v>248</v>
       </c>
       <c r="D115" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E115" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="E115" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="F115" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
@@ -4300,33 +4302,33 @@
         <v>248</v>
       </c>
       <c r="D116" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E116" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="E116" s="2" t="s">
-        <v>283</v>
-      </c>
       <c r="F116" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A117" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B117" s="32" t="s">
+      <c r="B117" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C117" s="32" t="s">
+      <c r="C117" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D117" s="32" t="s">
-        <v>284</v>
-      </c>
-      <c r="E117" s="32" t="s">
+      <c r="D117" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="E117" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="F117" s="32" t="s">
-        <v>322</v>
+      <c r="F117" s="2" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -4340,13 +4342,13 @@
         <v>248</v>
       </c>
       <c r="D118" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="E118" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="E118" s="2" t="s">
-        <v>286</v>
-      </c>
       <c r="F118" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -4360,10 +4362,10 @@
         <v>248</v>
       </c>
       <c r="D119" s="32" t="s">
+        <v>286</v>
+      </c>
+      <c r="E119" s="32" t="s">
         <v>287</v>
-      </c>
-      <c r="E119" s="32" t="s">
-        <v>288</v>
       </c>
       <c r="F119" s="32"/>
     </row>
@@ -4378,27 +4380,27 @@
         <v>248</v>
       </c>
       <c r="D120" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="E120" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="E120" s="2" t="s">
-        <v>290</v>
-      </c>
       <c r="F120" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="32" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="B121" s="32" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C121" s="32" t="s">
         <v>248</v>
       </c>
       <c r="D121" s="32" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E121" s="32"/>
       <c r="F121" s="32"/>

</xml_diff>

<commit_message>
Revert "Revert "Revert "feedback change"""
This reverts commit 9c4b50dcf2bd83bdbedf382030d543c24769c95d.
</commit_message>
<xml_diff>
--- a/Zacher/Feedback.xlsx
+++ b/Zacher/Feedback.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="327">
   <si>
     <t>Author</t>
   </si>
@@ -869,6 +869,9 @@
     <t>CLEAR ERC before you submit your work!!</t>
   </si>
   <si>
+    <t xml:space="preserve">Board outline oversized </t>
+  </si>
+  <si>
     <t>Used the space or reduce the size of the board. It is confusing if you have unused space letft there for some reason</t>
   </si>
   <si>
@@ -1007,6 +1010,9 @@
     <t>Took into consideration in the newest revision current revision.</t>
   </si>
   <si>
+    <t>smach comand and change all size at once would be cool</t>
+  </si>
+  <si>
     <t>schematic</t>
   </si>
   <si>
@@ -1017,12 +1023,6 @@
   </si>
   <si>
     <t>added a comment to call out the standard passives</t>
-  </si>
-  <si>
-    <t>group comand to make all the refrences the same size</t>
-  </si>
-  <si>
-    <t>Value removed</t>
   </si>
 </sst>
 </file>
@@ -1880,8 +1880,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A119" sqref="A119:F119"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -3600,7 +3600,7 @@
         <v>219</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -3620,7 +3620,7 @@
         <v>222</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -3700,7 +3700,7 @@
         <v>229</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -3720,7 +3720,7 @@
         <v>233</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
@@ -3740,7 +3740,7 @@
         <v>234</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -3760,7 +3760,7 @@
         <v>237</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.3">
@@ -3780,7 +3780,7 @@
         <v>239</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.3">
@@ -3800,7 +3800,7 @@
         <v>242</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="75" x14ac:dyDescent="0.3">
@@ -3820,7 +3820,7 @@
         <v>244</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.3">
@@ -3837,7 +3837,7 @@
         <v>245</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -3854,7 +3854,7 @@
         <v>246</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="37.5" x14ac:dyDescent="0.3">
@@ -3900,7 +3900,7 @@
         <v>250</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="112.5" x14ac:dyDescent="0.3">
@@ -3920,7 +3920,7 @@
         <v>252</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -3940,7 +3940,7 @@
         <v>254</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -3960,7 +3960,7 @@
         <v>256</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -3977,7 +3977,7 @@
         <v>257</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
@@ -3997,7 +3997,7 @@
         <v>259</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
@@ -4068,7 +4068,7 @@
         <v>263</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="105" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -4088,7 +4088,7 @@
         <v>263</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -4108,7 +4108,7 @@
         <v>268</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
@@ -4128,7 +4128,7 @@
         <v>270</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
@@ -4148,7 +4148,7 @@
         <v>272</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
@@ -4168,7 +4168,7 @@
         <v>274</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -4182,13 +4182,13 @@
         <v>248</v>
       </c>
       <c r="D110" s="36" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E110" s="36" t="s">
         <v>259</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
@@ -4202,13 +4202,13 @@
         <v>248</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="112" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -4222,34 +4222,32 @@
         <v>248</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B113" s="2" t="s">
+      <c r="B113" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="C113" s="2" t="s">
+      <c r="C113" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="D113" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="E113" s="2" t="s">
+      <c r="D113" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="E113" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="F113" s="2" t="s">
-        <v>326</v>
-      </c>
+      <c r="F113" s="32"/>
     </row>
     <row r="114" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A114" s="37" t="s">
@@ -4262,16 +4260,16 @@
         <v>248</v>
       </c>
       <c r="D114" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="E114" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="E114" s="2" t="s">
-        <v>277</v>
-      </c>
       <c r="F114" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A115" s="37" t="s">
         <v>1</v>
       </c>
@@ -4282,13 +4280,13 @@
         <v>248</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="56.25" x14ac:dyDescent="0.3">
@@ -4302,33 +4300,33 @@
         <v>248</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="117" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A117" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B117" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="D117" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="E117" s="2" t="s">
+      <c r="D117" s="32" t="s">
+        <v>284</v>
+      </c>
+      <c r="E117" s="32" t="s">
         <v>263</v>
       </c>
-      <c r="F117" s="2" t="s">
-        <v>325</v>
+      <c r="F117" s="32" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
@@ -4342,13 +4340,13 @@
         <v>248</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="119" spans="1:6" ht="37.5" x14ac:dyDescent="0.3">
@@ -4362,10 +4360,10 @@
         <v>248</v>
       </c>
       <c r="D119" s="32" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="E119" s="32" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="F119" s="32"/>
     </row>
@@ -4380,27 +4378,27 @@
         <v>248</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="32" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B121" s="32" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C121" s="32" t="s">
         <v>248</v>
       </c>
       <c r="D121" s="32" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E121" s="32"/>
       <c r="F121" s="32"/>

</xml_diff>